<commit_message>
fix: updated js file to meet CRUD requirement
</commit_message>
<xml_diff>
--- a/p4-node-app/checklists/Ckecklists.xlsx
+++ b/p4-node-app/checklists/Ckecklists.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\devving\projects\p4-node-app\Checklists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\devving\projects\p4-node-app\checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoints" sheetId="1" r:id="rId1"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -727,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: updated Checklist and  Endppoints
</commit_message>
<xml_diff>
--- a/p4-node-app/checklists/Ckecklists.xlsx
+++ b/p4-node-app/checklists/Ckecklists.xlsx
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
-  <si>
-    <t xml:space="preserve"># </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
   <si>
     <t>Action</t>
   </si>
@@ -181,18 +178,12 @@
     <t>Create</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
     <t>CREATE</t>
   </si>
   <si>
-    <t>Create  sample</t>
-  </si>
-  <si>
     <t>Read</t>
   </si>
   <si>
@@ -214,26 +205,122 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>Read  sample</t>
-  </si>
-  <si>
-    <t>Update  sample</t>
-  </si>
-  <si>
-    <t>Delete  sample</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Accomodation</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Flights</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>'/register'</t>
+  </si>
+  <si>
+    <t>'/login'</t>
+  </si>
+  <si>
+    <t>Create User</t>
+  </si>
+  <si>
+    <t>Read User</t>
+  </si>
+  <si>
+    <t>'/'</t>
+  </si>
+  <si>
+    <t>Create Accomodation</t>
+  </si>
+  <si>
+    <t>'/:id'</t>
+  </si>
+  <si>
+    <t>Display One Accommodation</t>
+  </si>
+  <si>
+    <t>/'</t>
+  </si>
+  <si>
+    <t>Display All Accommodation</t>
+  </si>
+  <si>
+    <t>Update an Accommodation</t>
+  </si>
+  <si>
+    <t>Delete an Accommodation</t>
+  </si>
+  <si>
+    <t>to follow</t>
+  </si>
+  <si>
+    <t>Create Event</t>
+  </si>
+  <si>
+    <t>Display One Event</t>
+  </si>
+  <si>
+    <t>Display All Event</t>
+  </si>
+  <si>
+    <t>Update an Event</t>
+  </si>
+  <si>
+    <t>Delete an Event</t>
+  </si>
+  <si>
+    <t>Create Flight</t>
+  </si>
+  <si>
+    <t>Display Flight</t>
+  </si>
+  <si>
+    <t>Display All Flight</t>
+  </si>
+  <si>
+    <t>Update a Flight</t>
+  </si>
+  <si>
+    <t>Delete a Flight</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Display User</t>
+  </si>
+  <si>
+    <t>Display All User</t>
+  </si>
+  <si>
+    <t>Update a User</t>
+  </si>
+  <si>
+    <t>Delete a User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,19 +336,28 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="8"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -273,7 +369,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -296,11 +392,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -308,17 +448,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -601,134 +765,658 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.41796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.47265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.15625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.20703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.9453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="3"/>
+    <col min="1" max="1" width="12.05078125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.41796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.05078125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.41796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.47265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83984375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="12.6" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="11"/>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="11"/>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="11"/>
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="11"/>
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="11"/>
+      <c r="B10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="11"/>
+      <c r="B11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="11"/>
+      <c r="B12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="11"/>
+      <c r="B15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="11"/>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F19" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="11"/>
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="11"/>
+      <c r="B22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="11"/>
+      <c r="B27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="11"/>
+      <c r="B28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F29" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="11"/>
+      <c r="B30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="11"/>
+      <c r="B31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="11"/>
+      <c r="B32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="11"/>
+      <c r="B33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
+      <c r="E33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -737,57 +1425,81 @@
     <col min="2" max="2" width="57.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +1513,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -810,45 +1522,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>16</v>
+      <c r="A1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adding READ.md file
</commit_message>
<xml_diff>
--- a/p4-node-app/checklists/Ckecklists.xlsx
+++ b/p4-node-app/checklists/Ckecklists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoints" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="68">
   <si>
     <t>Action</t>
   </si>
@@ -454,9 +454,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,15 +461,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -484,6 +472,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,19 +767,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.05078125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.41796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.05078125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.41796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.47265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="8"/>
+    <col min="1" max="1" width="12.05078125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.05078125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.41796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.47265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83984375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -803,596 +803,596 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
-      <c r="B10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
-      <c r="B13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="11"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="11"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" s="11"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A18" s="11"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" s="11"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" s="11"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" s="11"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="11"/>
-      <c r="B25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" s="11"/>
-      <c r="B27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28" s="11"/>
-      <c r="B28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32" s="11"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A33" s="11"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="13"/>
+      <c r="B33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1490,6 +1490,9 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1512,8 +1515,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
fix: updating READ.md file
</commit_message>
<xml_diff>
--- a/p4-node-app/checklists/Ckecklists.xlsx
+++ b/p4-node-app/checklists/Ckecklists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9156"/>
   </bookViews>
   <sheets>
     <sheet name="Endpoints" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="69">
   <si>
     <t>Action</t>
   </si>
@@ -315,12 +315,15 @@
   <si>
     <t>Delete a User</t>
   </si>
+  <si>
+    <t>Defining the Endpoints</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +363,12 @@
       <sz val="8"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -369,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -436,11 +445,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -484,6 +502,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
@@ -782,101 +803,92 @@
     <col min="7" max="16384" width="8.83984375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.65">
+      <c r="A1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="15"/>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="15"/>
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="I5" s="5"/>
     </row>
@@ -885,77 +897,78 @@
       <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>48</v>
+      <c r="C6" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="13"/>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1027,42 +1040,41 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="13"/>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="I15" s="5"/>
     </row>
@@ -1071,91 +1083,92 @@
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>48</v>
+      <c r="C16" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="13"/>
+      <c r="B19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="12" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="13"/>
-      <c r="B20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -1163,77 +1176,77 @@
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>48</v>
+      <c r="C21" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="13"/>
       <c r="B22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="13"/>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="13"/>
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="13"/>
       <c r="B25" s="5" t="s">
         <v>52</v>
       </c>
@@ -1305,41 +1318,41 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30" s="13"/>
-      <c r="B30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -1347,64 +1360,83 @@
       <c r="B31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>48</v>
+      <c r="C31" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="13"/>
       <c r="B32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="13"/>
       <c r="B33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" s="13"/>
+      <c r="B34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A18"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1515,7 +1547,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>